<commit_message>
Included simple verification datasets
</commit_message>
<xml_diff>
--- a/feature_selection_feat/poisson2d_data.xlsx
+++ b/feature_selection_feat/poisson2d_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\repos\bandgap\feature_selection_feat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F6AF3D-3915-45F5-8052-B16C6234A9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC5667A-BDCA-457D-82E8-215D7BA24196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E02FCFDB-5EA6-4C63-A570-62ECD074F549}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>x</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>u</t>
+  </si>
+  <si>
+    <t>best guess</t>
   </si>
 </sst>
 </file>
@@ -395,15 +398,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87EF6DA-E447-4A86-A453-D774B0049FD0}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,8 +419,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -425,8 +434,12 @@
         <f>SIN(PI()*A2)*SIN(PI()*B2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>(0.3302*SIN(2.043*B2)*TANH(1.2639*A2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -437,8 +450,12 @@
         <f t="shared" ref="C3:C66" si="0">SIN(PI()*A3)*SIN(PI()*B3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="1">(0.3302*SIN(2.043*B3)*TANH(1.2639*A3))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -449,8 +466,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -461,8 +482,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -473,8 +498,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -485,8 +514,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -497,8 +530,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -509,8 +546,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -521,8 +562,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.25</v>
       </c>
@@ -533,8 +578,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.25</v>
       </c>
@@ -545,8 +594,12 @@
         <f t="shared" si="0"/>
         <v>0.49999999999999989</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>4.9370020715151168E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.25</v>
       </c>
@@ -557,8 +610,12 @@
         <f t="shared" si="0"/>
         <v>0.70710678118654746</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>8.6138652628543158E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.25</v>
       </c>
@@ -569,8 +626,12 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0.10092093256337847</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.25</v>
       </c>
@@ -580,8 +641,12 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>8.9943776082239857E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.25</v>
       </c>
@@ -592,8 +657,12 @@
         <f t="shared" si="0"/>
         <v>-0.49999999999999989</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>5.6009033675624077E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.25</v>
       </c>
@@ -604,8 +673,12 @@
         <f t="shared" si="0"/>
         <v>-0.70710678118654746</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>7.7783359598227707E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.25</v>
       </c>
@@ -616,8 +689,12 @@
         <f t="shared" si="0"/>
         <v>-0.50000000000000011</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>-4.2437733328454914E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.25</v>
       </c>
@@ -627,8 +704,12 @@
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>-8.1821836784214355E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.5</v>
       </c>
@@ -639,8 +720,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.5</v>
       </c>
@@ -651,8 +736,12 @@
         <f t="shared" si="0"/>
         <v>0.70710678118654746</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>9.0292941775551416E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.5</v>
       </c>
@@ -663,8 +752,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>0.15753917526768615</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.5</v>
       </c>
@@ -675,8 +768,12 @@
         <f t="shared" si="0"/>
         <v>0.70710678118654757</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>0.18457452024286805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.5</v>
       </c>
@@ -686,8 +783,12 @@
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>0.16449837409880963</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.5</v>
       </c>
@@ -698,8 +799,12 @@
         <f t="shared" si="0"/>
         <v>-0.70710678118654746</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>0.1024350474907946</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.5</v>
       </c>
@@ -710,8 +815,12 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>1.4225816107778491E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.5</v>
       </c>
@@ -722,8 +831,12 @@
         <f t="shared" si="0"/>
         <v>-0.70710678118654768</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>-7.7614465803466995E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.5</v>
       </c>
@@ -733,8 +846,12 @@
       <c r="C28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>-0.14964414107402743</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.75</v>
       </c>
@@ -745,8 +862,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.75</v>
       </c>
@@ -757,8 +878,12 @@
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>0.11925815929938273</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.75</v>
       </c>
@@ -769,8 +894,12 @@
         <f t="shared" si="0"/>
         <v>0.70710678118654757</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>0.20807641982326314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.75</v>
       </c>
@@ -781,8 +910,12 @@
         <f t="shared" si="0"/>
         <v>0.50000000000000011</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>0.24378447644831616</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.75</v>
       </c>
@@ -792,8 +925,12 @@
       <c r="C33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>0.21726807120240699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.75</v>
       </c>
@@ -804,8 +941,12 @@
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>0.13529535056974737</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.75</v>
       </c>
@@ -816,8 +957,12 @@
         <f t="shared" si="0"/>
         <v>-0.70710678118654757</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>1.8789338459726038E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.75</v>
       </c>
@@ -828,8 +973,12 @@
         <f t="shared" si="0"/>
         <v>-0.50000000000000011</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>-0.10251253469773033</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.75</v>
       </c>
@@ -839,8 +988,12 @@
       <c r="C37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>-0.19764872495557448</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -851,8 +1004,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -862,8 +1019,12 @@
       <c r="C39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>0.13754511841525058</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -873,8 +1034,12 @@
       <c r="C40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>0.23998270619090678</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -884,8 +1049,12 @@
       <c r="C41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>0.28116621016015525</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -895,8 +1064,12 @@
       <c r="C42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>0.25058379868473152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -906,8 +1079,12 @@
       <c r="C43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>0.15604144089154212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -917,8 +1094,12 @@
       <c r="C44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>2.1670481907233464E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -928,8 +1109,12 @@
       <c r="C45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>-0.11823173195764547</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -939,8 +1124,12 @@
       <c r="C46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>-0.22795603620203198</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1.25</v>
       </c>
@@ -951,8 +1140,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1.25</v>
       </c>
@@ -963,8 +1156,12 @@
         <f t="shared" si="0"/>
         <v>-0.49999999999999989</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>0.14827041648746864</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1.25</v>
       </c>
@@ -975,8 +1172,12 @@
         <f t="shared" si="0"/>
         <v>-0.70710678118654746</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>0.25869573712744942</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1.25</v>
       </c>
@@ -987,8 +1188,12 @@
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>0.30309058993130389</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1.25</v>
       </c>
@@ -998,8 +1203,12 @@
       <c r="C51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>0.27012346656918934</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1.25</v>
       </c>
@@ -1010,8 +1219,12 @@
         <f t="shared" si="0"/>
         <v>0.49999999999999989</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>0.16820901895220136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1.25</v>
       </c>
@@ -1022,8 +1235,12 @@
         <f t="shared" si="0"/>
         <v>0.70710678118654746</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>2.3360271995762821E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1.25</v>
       </c>
@@ -1034,8 +1251,12 @@
         <f t="shared" si="0"/>
         <v>0.50000000000000011</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>-0.12745103818567177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1.25</v>
       </c>
@@ -1045,8 +1266,12 @@
       <c r="C55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>-0.24573126853159344</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1.5</v>
       </c>
@@ -1057,8 +1282,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1.5</v>
       </c>
@@ -1069,8 +1298,12 @@
         <f t="shared" si="0"/>
         <v>-0.70710678118654746</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>0.15429083297543253</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1.5</v>
       </c>
@@ -1081,8 +1314,12 @@
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>0.26919989647402887</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1.5</v>
       </c>
@@ -1093,8 +1330,12 @@
         <f t="shared" si="0"/>
         <v>-0.70710678118654757</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>0.31539737120431227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1.5</v>
       </c>
@@ -1104,8 +1345,12 @@
       <c r="C60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>0.28109164087155641</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1.5</v>
       </c>
@@ -1116,8 +1361,12 @@
         <f t="shared" si="0"/>
         <v>0.70710678118654746</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>0.17503902843834629</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1.5</v>
       </c>
@@ -1128,8 +1377,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>2.4308799490446821E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1.5</v>
       </c>
@@ -1140,8 +1393,12 @@
         <f t="shared" si="0"/>
         <v>0.70710678118654768</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>-0.13262609838904005</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1.5</v>
       </c>
@@ -1151,8 +1408,12 @@
       <c r="C64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>-0.25570901470458623</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1.75</v>
       </c>
@@ -1163,8 +1424,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1.75</v>
       </c>
@@ -1175,8 +1440,12 @@
         <f t="shared" si="0"/>
         <v>-0.50000000000000011</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>0.15758728908532404</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1.75</v>
       </c>
@@ -1184,11 +1453,15 @@
         <v>0.5</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C74" si="1">SIN(PI()*A67)*SIN(PI()*B67)</f>
+        <f t="shared" ref="C67:C74" si="2">SIN(PI()*A67)*SIN(PI()*B67)</f>
         <v>-0.70710678118654768</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <f t="shared" ref="D67:D82" si="3">(0.3302*SIN(2.043*B67)*TANH(1.2639*A67))</f>
+        <v>0.2749514089028669</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1.75</v>
       </c>
@@ -1196,11 +1469,15 @@
         <v>0.75</v>
       </c>
       <c r="C68">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-0.50000000000000011</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <f t="shared" si="3"/>
+        <v>0.32213590240088519</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1.75</v>
       </c>
@@ -1210,8 +1487,12 @@
       <c r="C69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <f t="shared" si="3"/>
+        <v>0.2870972229215154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1.75</v>
       </c>
@@ -1219,11 +1500,15 @@
         <v>1.25</v>
       </c>
       <c r="C70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.50000000000000011</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <f t="shared" si="3"/>
+        <v>0.17877877410980128</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1.75</v>
       </c>
@@ -1231,11 +1516,15 @@
         <v>1.5</v>
       </c>
       <c r="C71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.70710678118654768</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <f t="shared" si="3"/>
+        <v>2.4828162106223035E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1.75</v>
       </c>
@@ -1243,11 +1532,15 @@
         <v>1.75</v>
       </c>
       <c r="C72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.50000000000000022</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <f t="shared" si="3"/>
+        <v>-0.13545968288615168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1.75</v>
       </c>
@@ -1257,8 +1550,12 @@
       <c r="C73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <f t="shared" si="3"/>
+        <v>-0.2611722916058879</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2</v>
       </c>
@@ -1266,11 +1563,15 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2</v>
       </c>
@@ -1280,8 +1581,12 @@
       <c r="C75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <f t="shared" si="3"/>
+        <v>0.15936771255287627</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -1291,8 +1596,12 @@
       <c r="C76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <f t="shared" si="3"/>
+        <v>0.27805781389078543</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2</v>
       </c>
@@ -1302,8 +1611,12 @@
       <c r="C77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <f t="shared" si="3"/>
+        <v>0.32577539847766018</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2</v>
       </c>
@@ -1313,8 +1626,12 @@
       <c r="C78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <f t="shared" si="3"/>
+        <v>0.29034085149159489</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2</v>
       </c>
@@ -1324,8 +1641,12 @@
       <c r="C79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <f t="shared" si="3"/>
+        <v>0.18079861928115243</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2</v>
       </c>
@@ -1335,8 +1656,12 @@
       <c r="C80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <f t="shared" si="3"/>
+        <v>2.5108671040202955E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2</v>
       </c>
@@ -1346,8 +1671,12 @@
       <c r="C81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <f t="shared" si="3"/>
+        <v>-0.13699010833935624</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2</v>
       </c>
@@ -1356,6 +1685,10 @@
       </c>
       <c r="C82">
         <v>0</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="3"/>
+        <v>-0.26412301992762294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>